<commit_message>
updates to historic la county voter turnout...:
</commit_message>
<xml_diff>
--- a/data/la-county-voter-turnout-historic/_historic_turnout_la_county.xlsx
+++ b/data/la-county-voter-turnout-historic/_historic_turnout_la_county.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amendelson/Desktop/projects/elex_turnout_registration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckeller/_programming/2kpcc/_projects/kpcc_data_team/data/la-county-voter-turnout-historic/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="1700" windowWidth="28360" windowHeight="17060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="_historic_turnout_la_county" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -684,7 +687,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -825,7 +828,7 @@
         <v>2026068</v>
       </c>
       <c r="I3" s="13">
-        <f t="shared" ref="I2:M65" si="1">(H3-H4)/H4</f>
+        <f t="shared" ref="I3:M65" si="1">(H3-H4)/H4</f>
         <v>0.33396188526074261</v>
       </c>
       <c r="J3" s="13">

</xml_diff>